<commit_message>
updated BOM, fixed some typos
</commit_message>
<xml_diff>
--- a/TubeAmp.bom.xlsx
+++ b/TubeAmp.bom.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\tfa98xx_bt_spkr\kicad5_workspace\projects\TubeAmp_Rev1.2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\tubeamp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666BE5BC-1767-4F1A-B0BE-E2AD8E40A11E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD472D4-CDCD-4485-B3F5-53A3E203D1D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,279 +16,118 @@
     <sheet name="TubeAmp.bom" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="81">
   <si>
     <t>Link</t>
   </si>
   <si>
-    <t>C1</t>
-  </si>
-  <si>
     <t>CAP 1000UF/25V 10MM P7.5MM</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/32829549030.html?spm=a2g0s.9042311.0.0.27424c4d3Np1WM</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
     <t>CAP 1.5UF/63V 7.2X6MM P5MM</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/4000461563828.html?spm=a2g0s.9042311.0.0.27424c4d3Np1WM</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>C6</t>
-  </si>
-  <si>
     <t>CAP 47NF/100V 7X3.5MM P5MM</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/32847371848.html?spm=a2g0s.9042311.0.0.27424c4d3Np1WM</t>
-  </si>
-  <si>
-    <t>C7</t>
-  </si>
-  <si>
-    <t>C8</t>
-  </si>
-  <si>
     <t>CAP 100UF/25V 6.3MM P2.5MM</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/32803248529.html?spm=a2g0s.9042311.0.0.27424c4d3Np1WM</t>
-  </si>
-  <si>
-    <t>C9</t>
-  </si>
-  <si>
-    <t>C10</t>
-  </si>
-  <si>
     <t>CAP 470UF/16V 8MM P3.5MM</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/32864102646.html?spm=a2g0s.9042311.0.0.27424c4d3Np1WM</t>
-  </si>
-  <si>
-    <t>C11</t>
-  </si>
-  <si>
-    <t>C12</t>
-  </si>
-  <si>
     <t>CAP 47UF/25V 5MM P2.5MM</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/32911787493.html?spm=a2g0s.9042311.0.0.27424c4d3Np1WM</t>
-  </si>
-  <si>
-    <t>C13</t>
-  </si>
-  <si>
-    <t>C14</t>
-  </si>
-  <si>
-    <t>CAP 47NF/50V 4.6X3MM P2.5MM</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/32865098104.html?spm=a2g0s.9042311.0.0.27424c4d3Np1WM</t>
-  </si>
-  <si>
-    <t>C15</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
     <t>LED BLUE 3MM</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/32890682652.html?spm=a2g0o.productlist.0.0.61623afcPWcv7S</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
     <t>DC BARREL JACK 5.5X2.1MM</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/33005175186.html?spm=a2g0o.productlist.0.0.21f1579clrh5Wc</t>
-  </si>
-  <si>
-    <t>J2</t>
-  </si>
-  <si>
     <t>AUDIO JACK 3.5" PJ-320A</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/33029465106.html?spm=a2g0s.9042311.0.0.27424c4dxqRJoG</t>
-  </si>
-  <si>
-    <t>J3</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
     <t>IRF510 POWER N-MOS TO-220</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/32715627674.html?spm=a2g0o.productlist.0.0.31ea55b06h7Yqs</t>
-  </si>
-  <si>
-    <t>Q2</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
     <t>RES 3.3K OHM 1/8W 3.6MM</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/32625241391.html?spm=a2g0s.9042311.0.0.27424c4dhgKCJy</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
     <t>RES 2K OHM 1/8W 3.6MM</t>
   </si>
   <si>
-    <t>R3</t>
-  </si>
-  <si>
     <t>R4</t>
   </si>
   <si>
     <t>RES 5.6 OHM 1/4W 6.3MM</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/32909364829.html?spm=a2g0o.productlist.0.0.2a8159c0hc4SB8</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
     <t>RES 10 OHM 1/8W 3.6MM</t>
   </si>
   <si>
-    <t>R6</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
     <t>RES 100K OHM 1/8W 3.6MM</t>
   </si>
   <si>
-    <t>R8</t>
-  </si>
-  <si>
-    <t>R9</t>
-  </si>
-  <si>
     <t>RES 100 OHM 1/8W 3.6MM</t>
   </si>
   <si>
-    <t>R10</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
     <t>RES 150 OHM 1/4W 6.3MM</t>
   </si>
   <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>R13</t>
-  </si>
-  <si>
     <t>RES 10 OHM 3W 15.5MM</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/4000773914003.html?spm=a2g0o.productlist.0.0.631869f95uFNMO</t>
-  </si>
-  <si>
-    <t>R14</t>
-  </si>
-  <si>
-    <t>R15</t>
-  </si>
-  <si>
     <t>RES 1K OHM 1/4W 6.3MM</t>
   </si>
   <si>
-    <t>R16</t>
-  </si>
-  <si>
     <t>RV1</t>
   </si>
   <si>
     <t>POT DUAL RK097G-B50K</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/1907441292.html?spm=a2g0s.9042311.0.0.27424c4d3HgVjv</t>
-  </si>
-  <si>
-    <t>RV2</t>
-  </si>
-  <si>
     <t>POT 20K OHM 3296W</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/32845414733.html?spm=a2g0s.9042311.0.0.27424c4dXXN7yO</t>
-  </si>
-  <si>
-    <t>RV3</t>
-  </si>
-  <si>
     <t>SW1</t>
   </si>
   <si>
     <t>SWITCH ON/OFF PUSH BUTTON RIGHT ANGLE 5.8X5.8MM</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/4000316236780.html?spm=a2g0s.9042311.0.0.27424c4duEjEGY</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
     <t>12AU7/ECC82 SOCKET GZC9-A-G</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/4000219880005.html?spm=a2g0s.9042311.0.0.27424c4d0ksM9X</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
     <t>LM317 VOLTAGE REGULATOR TO-220</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/32549487669.html?spm=a2g0s.9042311.0.0.27424c4dxSu9Eg</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
     <t>Reference</t>
   </si>
   <si>
@@ -304,26 +143,146 @@
     <t>HEATSINK WITH SCREW FOR TO-220</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/32802123591.html?spm=a2g0s.9042311.0.0.27424c4dcq73ld</t>
-  </si>
-  <si>
     <t>VACUUM TUBE 12AU7</t>
   </si>
   <si>
     <t>KNOB</t>
   </si>
   <si>
-    <t>POTENTIOMETER KNOB 15MM</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/32976364232.html?spm=a2g0s.9042311.0.0.27424c4dz623hb</t>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>C1, C2, C3</t>
+  </si>
+  <si>
+    <t>U2, U3</t>
+  </si>
+  <si>
+    <t>R13, R14</t>
+  </si>
+  <si>
+    <t>R11, R12</t>
+  </si>
+  <si>
+    <t>R15, R16</t>
+  </si>
+  <si>
+    <t>C4, C5</t>
+  </si>
+  <si>
+    <t>R9, R10</t>
+  </si>
+  <si>
+    <t>R5, R6</t>
+  </si>
+  <si>
+    <t>R7, R8</t>
+  </si>
+  <si>
+    <t>R2, R3</t>
+  </si>
+  <si>
+    <t>POTENTIOMETER KNOB</t>
+  </si>
+  <si>
+    <t>RV2, RV3</t>
+  </si>
+  <si>
+    <t>J2, J3</t>
+  </si>
+  <si>
+    <t>Q1, Q2</t>
+  </si>
+  <si>
+    <t>C14, C15</t>
+  </si>
+  <si>
+    <t>C12, C13</t>
+  </si>
+  <si>
+    <t>C10, C11</t>
+  </si>
+  <si>
+    <t>C8, C9</t>
+  </si>
+  <si>
+    <t>C6, C7</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32874772300.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32829549030.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/4000461563828.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32890682652.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32847371848.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32803248529.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32864102646.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32911787493.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32865098104.html</t>
+  </si>
+  <si>
+    <t>CAP 100NF/50V 4.6X3MM P2.5MM</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/33005175186.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32715627674.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32909364829.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/4000773914003.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/1907441292.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32845414733.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/4000316236780.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/4000219880005.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32549487669.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32816123723.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32802123591.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/33005178438.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00"/>
+  </numFmts>
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -454,6 +413,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -756,7 +723,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -799,8 +766,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -808,11 +776,20 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -846,6 +823,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1166,550 +1144,465 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:XFD46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="1"/>
-    <col min="2" max="2" width="51.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="91.28515625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="13" style="1"/>
+    <col min="2" max="2" width="11.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="51.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="52.7109375" style="1" customWidth="1"/>
+    <col min="5" max="6" width="13" style="4"/>
+    <col min="7" max="7" width="13" style="1"/>
+    <col min="8" max="9" width="13" style="4"/>
+    <col min="10" max="16384" width="13" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="1">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="1">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D7" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="D9" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="D10" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D11" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="D12" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="D13" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D14" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="D15" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="D16" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D17" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="D18" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="D19" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="D20" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D21" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="D22" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="D23" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="D24" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="D25" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="1" t="s">
+      <c r="D26" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="B28" s="1">
+        <v>4</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="D28" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B42" s="1" t="s">
+      <c r="D29" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>98</v>
-      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I30" s="6"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D10" r:id="rId1" xr:uid="{53E75DF8-35C6-4965-A328-EC838518C136}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{8EEEBB79-320D-41A3-BD9C-B3D9C3941171}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{32A954AA-2A66-4E0A-ACF1-86C3FDA305E5}"/>
+    <hyperlink ref="D25" r:id="rId4" xr:uid="{2A749DDF-9442-4E99-8CCC-65F20EEDC3C2}"/>
+    <hyperlink ref="D24" r:id="rId5" xr:uid="{7B195FB9-75C3-4AFE-8BDB-5A485D853108}"/>
+    <hyperlink ref="D26" r:id="rId6" xr:uid="{80C9D1A5-652A-40C4-9BFB-A35E956A4A4C}"/>
+    <hyperlink ref="D28" r:id="rId7" xr:uid="{AF8129BF-3099-49E8-8203-94F3CD349C9C}"/>
+    <hyperlink ref="D15" r:id="rId8" xr:uid="{4150677A-53F7-4BF9-85FA-CD95D928F572}"/>
+    <hyperlink ref="D19" r:id="rId9" xr:uid="{127D3676-5FC0-4905-B531-2BE0AB7B97B6}"/>
+    <hyperlink ref="D21" r:id="rId10" xr:uid="{38A3D735-82C8-457B-9313-A7639BB4D555}"/>
+    <hyperlink ref="D27" r:id="rId11" xr:uid="{2AAB32D6-F546-4CF6-B5BA-3575B0B6B7E8}"/>
+    <hyperlink ref="D16" r:id="rId12" xr:uid="{0CD43EA2-275A-4157-BF86-061FFC92E4FC}"/>
+    <hyperlink ref="D17" r:id="rId13" xr:uid="{5012AF2E-9F32-4A7D-8E3D-A265011D7802}"/>
+    <hyperlink ref="D18" r:id="rId14" xr:uid="{A97C5211-C75C-4AE1-9322-2DB3709D449C}"/>
+    <hyperlink ref="D14" r:id="rId15" xr:uid="{36945B20-1C09-4A9D-85DC-D28FC953FB9E}"/>
+    <hyperlink ref="D13" r:id="rId16" xr:uid="{63A807F8-1117-4A6D-A15F-40422F57556A}"/>
+    <hyperlink ref="D29" r:id="rId17" xr:uid="{841000FF-5052-41B7-B521-42296E128041}"/>
+    <hyperlink ref="D22" r:id="rId18" xr:uid="{EF9CCAA6-DEEC-432C-A2A4-5EFE73B6437C}"/>
+    <hyperlink ref="D23" r:id="rId19" xr:uid="{3FF0D189-1FAD-4A80-9AA6-F06CB88DBED3}"/>
+    <hyperlink ref="D20" r:id="rId20" xr:uid="{4FFE3B73-19C6-426C-A135-20095E424D90}"/>
+    <hyperlink ref="D9" r:id="rId21" xr:uid="{A32F5739-5170-4318-82D9-1A9DC41DD668}"/>
+    <hyperlink ref="D12" r:id="rId22" xr:uid="{175CEE37-8486-419F-880A-1BE8C96F180F}"/>
+    <hyperlink ref="D11" r:id="rId23" xr:uid="{E92A2F6C-61CD-4BD6-8345-EB3C718F410C}"/>
+    <hyperlink ref="D4" r:id="rId24" xr:uid="{9645F5A7-A158-4DE0-978C-D98B301A0F16}"/>
+    <hyperlink ref="D5" r:id="rId25" xr:uid="{3261B47A-FC00-479D-B66A-BE3C20F72E06}"/>
+    <hyperlink ref="D6" r:id="rId26" xr:uid="{E7793935-6A17-495A-8616-A7DB80B2DE63}"/>
+    <hyperlink ref="D7" r:id="rId27" xr:uid="{FDBC7A8F-4AFE-45C6-8BD4-4ED4E8774A7E}"/>
+    <hyperlink ref="D8" r:id="rId28" xr:uid="{44173A04-25A4-4F18-9664-9DF961FC7EF7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated value of C6/C7, frequency response is now flat between 20Hz and 20kHz
</commit_message>
<xml_diff>
--- a/TubeAmp.bom.xlsx
+++ b/TubeAmp.bom.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\tubeamp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD472D4-CDCD-4485-B3F5-53A3E203D1D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59671C3-0FDE-40D7-9206-CC9A76B60A4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>CAP 1.5UF/63V 7.2X6MM P5MM</t>
   </si>
   <si>
-    <t>CAP 47NF/100V 7X3.5MM P5MM</t>
-  </si>
-  <si>
     <t>CAP 100UF/25V 6.3MM P2.5MM</t>
   </si>
   <si>
@@ -221,9 +218,6 @@
     <t>https://www.aliexpress.com/item/32890682652.html</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/32847371848.html</t>
-  </si>
-  <si>
     <t>https://www.aliexpress.com/item/32803248529.html</t>
   </si>
   <si>
@@ -273,6 +267,12 @@
   </si>
   <si>
     <t>https://www.aliexpress.com/item/33005178438.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32380844991.html</t>
+  </si>
+  <si>
+    <t>CAP 1.5NF/100V 7X3.5MM P5MM</t>
   </si>
 </sst>
 </file>
@@ -1147,7 +1147,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,13 +1164,13 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -1178,7 +1178,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1">
         <v>3</v>
@@ -1187,12 +1187,12 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -1201,371 +1201,371 @@
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>3</v>
+        <v>80</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="1">
         <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="1">
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" s="1">
         <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" s="1">
         <v>2</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" s="1">
         <v>2</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17" s="1">
         <v>2</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" s="1">
         <v>2</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" s="1">
         <v>2</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="1">
         <v>2</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21" s="1">
         <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="1">
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B23" s="1">
         <v>2</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" s="1">
         <v>1</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" s="1">
         <v>1</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" s="1">
         <v>2</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="1">
         <v>1</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="1">
         <v>4</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="1">
         <v>1</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Rev1.3, changed R9/R10/C6/C7 value, added 1MOhm resistors in parallel to C6/C7
</commit_message>
<xml_diff>
--- a/TubeAmp.bom.xlsx
+++ b/TubeAmp.bom.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\tubeamp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59671C3-0FDE-40D7-9206-CC9A76B60A4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA97486C-B76D-44EC-AAA6-17495144774C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,249 +30,252 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="81">
-  <si>
-    <t>Link</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="82">
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1 C2 C3 </t>
   </si>
   <si>
     <t>CAP 1000UF/25V 10MM P7.5MM</t>
   </si>
   <si>
+    <t>https://www.aliexpress.com/item/32829549030.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C10 C11 </t>
+  </si>
+  <si>
+    <t>CAP 470UF/16V 8MM P3.5MM</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32864102646.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C12 C13 </t>
+  </si>
+  <si>
+    <t>CAP 47UF/25V 5MM P2.5MM</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32911787493.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C14 C15 </t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32865098104.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C4 C5 </t>
+  </si>
+  <si>
     <t>CAP 1.5UF/63V 7.2X6MM P5MM</t>
   </si>
   <si>
+    <t>https://www.aliexpress.com/item/4000461563828.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C7 C6 </t>
+  </si>
+  <si>
+    <t>CAP 68PF/50V 7X3.5MM P5MM</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32813120619.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9 C8 </t>
+  </si>
+  <si>
     <t>CAP 100UF/25V 6.3MM P2.5MM</t>
   </si>
   <si>
-    <t>CAP 470UF/16V 8MM P3.5MM</t>
-  </si>
-  <si>
-    <t>CAP 47UF/25V 5MM P2.5MM</t>
-  </si>
-  <si>
-    <t>D1</t>
+    <t>https://www.aliexpress.com/item/32803248529.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1 </t>
   </si>
   <si>
     <t>LED BLUE 3MM</t>
   </si>
   <si>
-    <t>J1</t>
+    <t>https://www.aliexpress.com/item/32890682652.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J1 </t>
   </si>
   <si>
     <t>DC BARREL JACK 5.5X2.1MM</t>
   </si>
   <si>
-    <t>AUDIO JACK 3.5" PJ-320A</t>
+    <t>https://www.aliexpress.com/item/33005175186.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J2 J3 </t>
+  </si>
+  <si>
+    <t>AUDIO JACK 3.5 PJ-320A"</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/33029465106.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1 Q2 </t>
   </si>
   <si>
     <t>IRF510 POWER N-MOS TO-220</t>
   </si>
   <si>
-    <t>R1</t>
+    <t>https://www.aliexpress.com/item/32715627674.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1 R2 </t>
+  </si>
+  <si>
+    <t>RES 2K OHM 1/8W 3.6MM</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/33007959640.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R11 R12 </t>
+  </si>
+  <si>
+    <t>RES 1M OHM 1/8W 3.6MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R13 R14 </t>
+  </si>
+  <si>
+    <t>RES 150 OHM 1/4W 6.3MM</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32909364829.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R15 R16 </t>
+  </si>
+  <si>
+    <t>RES 10 OHM 3W 15.5MM</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/4000773914003.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R17 R18 </t>
+  </si>
+  <si>
+    <t>RES 1K OHM 1/4W 6.3MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3 </t>
   </si>
   <si>
     <t>RES 3.3K OHM 1/8W 3.6MM</t>
   </si>
   <si>
-    <t>RES 2K OHM 1/8W 3.6MM</t>
-  </si>
-  <si>
-    <t>R4</t>
+    <t xml:space="preserve">R4 R5 </t>
+  </si>
+  <si>
+    <t>RES 10 OHM 1/8W 3.6MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6 </t>
   </si>
   <si>
     <t>RES 5.6 OHM 1/4W 6.3MM</t>
   </si>
   <si>
-    <t>RES 10 OHM 1/8W 3.6MM</t>
+    <t xml:space="preserve">R7 R8 R9 R10 </t>
   </si>
   <si>
     <t>RES 100K OHM 1/8W 3.6MM</t>
   </si>
   <si>
-    <t>RES 100 OHM 1/8W 3.6MM</t>
-  </si>
-  <si>
-    <t>RES 150 OHM 1/4W 6.3MM</t>
-  </si>
-  <si>
-    <t>RES 10 OHM 3W 15.5MM</t>
-  </si>
-  <si>
-    <t>RES 1K OHM 1/4W 6.3MM</t>
-  </si>
-  <si>
-    <t>RV1</t>
+    <t xml:space="preserve">RV1 </t>
   </si>
   <si>
     <t>POT DUAL RK097G-B50K</t>
   </si>
   <si>
+    <t>https://www.aliexpress.com/item/1907441292.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RV2 RV3 </t>
+  </si>
+  <si>
     <t>POT 20K OHM 3296W</t>
   </si>
   <si>
-    <t>SW1</t>
+    <t>https://www.aliexpress.com/item/32845414733.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW1 </t>
   </si>
   <si>
     <t>SWITCH ON/OFF PUSH BUTTON RIGHT ANGLE 5.8X5.8MM</t>
   </si>
   <si>
-    <t>U1</t>
+    <t>https://www.aliexpress.com/item/4000316236780.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U1 </t>
   </si>
   <si>
     <t>12AU7/ECC82 SOCKET GZC9-A-G</t>
   </si>
   <si>
+    <t>https://www.aliexpress.com/item/4000219880005.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U2 U3 </t>
+  </si>
+  <si>
     <t>LM317 VOLTAGE REGULATOR TO-220</t>
   </si>
   <si>
-    <t>Reference</t>
-  </si>
-  <si>
-    <t>Value</t>
+    <t>https://www.aliexpress.com/item/32549487669.html</t>
   </si>
   <si>
     <t>TUBE</t>
   </si>
   <si>
+    <t>VACUUM TUBE 12AU7</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32816123723.html</t>
+  </si>
+  <si>
     <t>HEATSINK</t>
   </si>
   <si>
     <t>HEATSINK WITH SCREW FOR TO-220</t>
   </si>
   <si>
-    <t>VACUUM TUBE 12AU7</t>
+    <t>https://www.aliexpress.com/item/32802123591.html</t>
   </si>
   <si>
     <t>KNOB</t>
   </si>
   <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>C1, C2, C3</t>
-  </si>
-  <si>
-    <t>U2, U3</t>
-  </si>
-  <si>
-    <t>R13, R14</t>
-  </si>
-  <si>
-    <t>R11, R12</t>
-  </si>
-  <si>
-    <t>R15, R16</t>
-  </si>
-  <si>
-    <t>C4, C5</t>
-  </si>
-  <si>
-    <t>R9, R10</t>
-  </si>
-  <si>
-    <t>R5, R6</t>
-  </si>
-  <si>
-    <t>R7, R8</t>
-  </si>
-  <si>
-    <t>R2, R3</t>
-  </si>
-  <si>
     <t>POTENTIOMETER KNOB</t>
   </si>
   <si>
-    <t>RV2, RV3</t>
-  </si>
-  <si>
-    <t>J2, J3</t>
-  </si>
-  <si>
-    <t>Q1, Q2</t>
-  </si>
-  <si>
-    <t>C14, C15</t>
-  </si>
-  <si>
-    <t>C12, C13</t>
-  </si>
-  <si>
-    <t>C10, C11</t>
-  </si>
-  <si>
-    <t>C8, C9</t>
-  </si>
-  <si>
-    <t>C6, C7</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/32874772300.html</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/32829549030.html</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/4000461563828.html</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/32890682652.html</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/32803248529.html</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/32864102646.html</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/32911787493.html</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/32865098104.html</t>
+    <t>https://www.aliexpress.com/item/33005178438.html</t>
   </si>
   <si>
     <t>CAP 100NF/50V 4.6X3MM P2.5MM</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/33005175186.html</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/32715627674.html</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/32909364829.html</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/4000773914003.html</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/1907441292.html</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/32845414733.html</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/4000316236780.html</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/4000219880005.html</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/32549487669.html</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/32816123723.html</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/32802123591.html</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/33005178438.html</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/32380844991.html</t>
-  </si>
-  <si>
-    <t>CAP 1.5NF/100V 7X3.5MM P5MM</t>
   </si>
 </sst>
 </file>
@@ -768,7 +771,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -776,16 +779,13 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1147,244 +1147,307 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" style="1"/>
-    <col min="2" max="2" width="11.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="51.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="52.7109375" style="1" customWidth="1"/>
-    <col min="5" max="6" width="13" style="4"/>
-    <col min="7" max="7" width="13" style="1"/>
-    <col min="8" max="9" width="13" style="4"/>
-    <col min="10" max="16384" width="13" style="1"/>
+    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1"/>
+    <col min="3" max="3" width="52.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="53.42578125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1">
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1">
         <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1">
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="B12" s="1">
         <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="B13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B14" s="1">
         <v>2</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="B15" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B16" s="1">
         <v>2</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -1394,215 +1457,272 @@
         <v>2</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B18" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B19" s="1">
         <v>2</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>69</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="B20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>70</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B21" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>69</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="B22" s="1">
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>71</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B23" s="1">
         <v>2</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>72</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="B24" s="1">
         <v>1</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>73</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="B25" s="1">
         <v>1</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>74</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="B26" s="1">
         <v>2</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>75</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="B27" s="1">
         <v>1</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>76</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="B28" s="1">
         <v>4</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>77</v>
       </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
       <c r="B29" s="1">
         <v>1</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>78</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I30" s="6"/>
+      <c r="I30" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" r:id="rId1" xr:uid="{53E75DF8-35C6-4965-A328-EC838518C136}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{8EEEBB79-320D-41A3-BD9C-B3D9C3941171}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{32A954AA-2A66-4E0A-ACF1-86C3FDA305E5}"/>
-    <hyperlink ref="D25" r:id="rId4" xr:uid="{2A749DDF-9442-4E99-8CCC-65F20EEDC3C2}"/>
-    <hyperlink ref="D24" r:id="rId5" xr:uid="{7B195FB9-75C3-4AFE-8BDB-5A485D853108}"/>
-    <hyperlink ref="D26" r:id="rId6" xr:uid="{80C9D1A5-652A-40C4-9BFB-A35E956A4A4C}"/>
-    <hyperlink ref="D28" r:id="rId7" xr:uid="{AF8129BF-3099-49E8-8203-94F3CD349C9C}"/>
-    <hyperlink ref="D15" r:id="rId8" xr:uid="{4150677A-53F7-4BF9-85FA-CD95D928F572}"/>
-    <hyperlink ref="D19" r:id="rId9" xr:uid="{127D3676-5FC0-4905-B531-2BE0AB7B97B6}"/>
-    <hyperlink ref="D21" r:id="rId10" xr:uid="{38A3D735-82C8-457B-9313-A7639BB4D555}"/>
-    <hyperlink ref="D27" r:id="rId11" xr:uid="{2AAB32D6-F546-4CF6-B5BA-3575B0B6B7E8}"/>
-    <hyperlink ref="D16" r:id="rId12" xr:uid="{0CD43EA2-275A-4157-BF86-061FFC92E4FC}"/>
-    <hyperlink ref="D17" r:id="rId13" xr:uid="{5012AF2E-9F32-4A7D-8E3D-A265011D7802}"/>
-    <hyperlink ref="D18" r:id="rId14" xr:uid="{A97C5211-C75C-4AE1-9322-2DB3709D449C}"/>
-    <hyperlink ref="D14" r:id="rId15" xr:uid="{36945B20-1C09-4A9D-85DC-D28FC953FB9E}"/>
-    <hyperlink ref="D13" r:id="rId16" xr:uid="{63A807F8-1117-4A6D-A15F-40422F57556A}"/>
-    <hyperlink ref="D29" r:id="rId17" xr:uid="{841000FF-5052-41B7-B521-42296E128041}"/>
-    <hyperlink ref="D22" r:id="rId18" xr:uid="{EF9CCAA6-DEEC-432C-A2A4-5EFE73B6437C}"/>
-    <hyperlink ref="D23" r:id="rId19" xr:uid="{3FF0D189-1FAD-4A80-9AA6-F06CB88DBED3}"/>
-    <hyperlink ref="D20" r:id="rId20" xr:uid="{4FFE3B73-19C6-426C-A135-20095E424D90}"/>
-    <hyperlink ref="D9" r:id="rId21" xr:uid="{A32F5739-5170-4318-82D9-1A9DC41DD668}"/>
-    <hyperlink ref="D12" r:id="rId22" xr:uid="{175CEE37-8486-419F-880A-1BE8C96F180F}"/>
-    <hyperlink ref="D11" r:id="rId23" xr:uid="{E92A2F6C-61CD-4BD6-8345-EB3C718F410C}"/>
-    <hyperlink ref="D4" r:id="rId24" xr:uid="{9645F5A7-A158-4DE0-978C-D98B301A0F16}"/>
-    <hyperlink ref="D5" r:id="rId25" xr:uid="{3261B47A-FC00-479D-B66A-BE3C20F72E06}"/>
-    <hyperlink ref="D6" r:id="rId26" xr:uid="{E7793935-6A17-495A-8616-A7DB80B2DE63}"/>
-    <hyperlink ref="D7" r:id="rId27" xr:uid="{FDBC7A8F-4AFE-45C6-8BD4-4ED4E8774A7E}"/>
-    <hyperlink ref="D8" r:id="rId28" xr:uid="{44173A04-25A4-4F18-9664-9DF961FC7EF7}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="D14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="D15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="D18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="D19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="D20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="D21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="D22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="D23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="D24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="D25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="D26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="D27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="D28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="D29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated R9/R10 value to 6.8kOhm
</commit_message>
<xml_diff>
--- a/TubeAmp.bom.xlsx
+++ b/TubeAmp.bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\tubeamp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA97486C-B76D-44EC-AAA6-17495144774C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211FF5EA-23D4-441A-8825-580DED0A446E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="810" windowWidth="21825" windowHeight="14790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TubeAmp.bom" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="84">
   <si>
     <t>Reference</t>
   </si>
@@ -197,9 +197,6 @@
     <t>RES 5.6 OHM 1/4W 6.3MM</t>
   </si>
   <si>
-    <t xml:space="preserve">R7 R8 R9 R10 </t>
-  </si>
-  <si>
     <t>RES 100K OHM 1/8W 3.6MM</t>
   </si>
   <si>
@@ -276,6 +273,15 @@
   </si>
   <si>
     <t>CAP 100NF/50V 4.6X3MM P2.5MM</t>
+  </si>
+  <si>
+    <t>RES 6.8K OHM 1/8W 3.6MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7 R8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R9 R10 </t>
   </si>
 </sst>
 </file>
@@ -1144,10 +1150,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E1" sqref="E1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1236,7 +1242,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>14</v>
@@ -1527,13 +1533,13 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="B21" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>38</v>
@@ -1546,34 +1552,35 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="B22" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
+      <c r="G22" s="4"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B23" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -1582,16 +1589,16 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B24" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -1600,16 +1607,16 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B25" s="1">
         <v>1</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -1618,16 +1625,16 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B26" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -1636,16 +1643,16 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B27" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -1654,16 +1661,16 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B28" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -1672,16 +1679,16 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B29" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -1689,7 +1696,25 @@
       <c r="I29" s="3"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="H30" s="3"/>
       <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I31" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1713,16 +1738,17 @@
     <hyperlink ref="D19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
     <hyperlink ref="D20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
     <hyperlink ref="D21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="D22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="D23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="D24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="D25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="D26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="D27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="D28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="D29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="D23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="D24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="D25" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="D26" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="D27" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="D28" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="D29" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="D30" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="D22" r:id="rId29" xr:uid="{E88ECAC1-6AFE-4E7B-A1AC-C82044D28C16}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId29"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>